<commit_message>
export excel as csv
</commit_message>
<xml_diff>
--- a/survey_data.xlsx
+++ b/survey_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kelley/Desktop/tfcb-homework01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96371EDE-DA5D-9443-BFA1-36BD833889E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5CE90E-CE99-A346-87AB-570935209896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1400" yWindow="500" windowWidth="25120" windowHeight="15580" tabRatio="481" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -591,7 +591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A247DA0A-05FC-A34A-B4B9-1C1E2F9F9C78}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>

</xml_diff>